<commit_message>
Adding SV39 and SV48 VM testplans
</commit_message>
<xml_diff>
--- a/testplans/DV plan SV39 Virtual Memory.xlsx
+++ b/testplans/DV plan SV39 Virtual Memory.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="89">
   <si>
     <t>Requirement
 Location</t>
@@ -130,9 +130,6 @@
   <si>
     <t>Flush all TLB entries as rs1 and rs2 is always 0. Check that:
 -TLB miss is recieved on the second access after running SFENCE</t>
-  </si>
-  <si>
-    <t>Vaddr assumed to be 64'd0</t>
   </si>
   <si>
     <t>mstatus.TVM</t>
@@ -491,7 +488,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -508,11 +505,6 @@
       <name val="Arial"/>
     </font>
     <font/>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -599,18 +591,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -628,36 +614,18 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -665,23 +633,14 @@
     <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -943,710 +902,708 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="10" t="s">
+      <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
+      <c r="G3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="7" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="10" t="s">
+      <c r="G4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="13"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="7" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="13"/>
+      <c r="G5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="9" t="s">
+      <c r="G6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="20" t="s">
+      <c r="K6" s="8"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="14"/>
+      <c r="B7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="22"/>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="C8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="23"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="25" t="s">
+      <c r="G8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="C9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="8"/>
+      <c r="L18" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="8"/>
+      <c r="L19" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="24"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="G20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="8"/>
+      <c r="L20" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="K21" s="8"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="G23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K24" s="8"/>
+      <c r="L24" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="5"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="5"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="12"/>
-      <c r="L17" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="12"/>
-      <c r="L18" s="26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="5"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" s="12"/>
-      <c r="L20" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" s="12"/>
-      <c r="L21" s="26"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="5"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="12"/>
-      <c r="L22" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" s="12"/>
-      <c r="L23" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="5"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K24" s="12"/>
-      <c r="L24" s="26" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1658,14 +1615,14 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I24">
       <formula1>"Testcase,Functional Coverage,Assertion Coverage,Code Coverage"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H24 J2:J24">
+      <formula1>"Done,To be Done,N/A"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F24">
       <formula1>"Self Checking,Signature Check,Check against RM,Assertion Check,Any/All,N/A"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G24">
       <formula1>"RISC-V Compliance,Directed Self-Checking,Directed Non-Self-Checking,Constrained-Random,ENV capability,not specific test,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H24 J2:J24">
-      <formula1>"Done,To be Done,N/A"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K2:K24">
       <formula1>"Covered,Not covered"</formula1>

</xml_diff>